<commit_message>
change date_time type to string 可以正常显示到网页
</commit_message>
<xml_diff>
--- a/erp_k/ERP设计思路.xlsx
+++ b/erp_k/ERP设计思路.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="407"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="407" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="思路" sheetId="1" r:id="rId1"/>
     <sheet name="步骤" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="统计表" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -146,8 +146,44 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>作者</author>
+  </authors>
+  <commentList>
+    <comment ref="I51" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+自己做单多少：拆分所得多少。</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="594">
   <si>
     <t>公司</t>
   </si>
@@ -2164,6 +2200,346 @@
   </si>
   <si>
     <t>zn_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QA经理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>九洲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生产经理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>large</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cmc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plant</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>small</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>quality</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>manufact</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kyle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shelley</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. 关于offer表和业绩表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>客户贡献</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不同类别offer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>只需要一张主表，进行不同搜索即可</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>raya</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>offer_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kevin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>amy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kyle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select offer表.name,offer.yeji,offer统计.时间 groupby name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1）行业，职能，部门表，业绩表，员工offer表：只需要额外2张表格即可搞定。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2）展示基础数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>追加图标功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1)估计要学习,pandas画图</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>明济</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PD ED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kyle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kerwin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>medical</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shelley</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>con_window</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kyle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>medical</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>瑞博</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>项目经理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>刘儿姐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>张三</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>铁柱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>钢弹</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>二波</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shelley</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>医学经理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kerwin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>炊鸭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kerwin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shelley</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shark</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>团队业绩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最佳客户经理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>合作拆分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>raya</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kyle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ygoffer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zoffer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yg_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hangye_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zhineng_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bumen_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>company</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cnd_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>client_offer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>offer_type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>team_offer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>offer_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>client_owner</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yg_yeji</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shelley</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>frank</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>frank</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>总表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kyle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>raya</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>amy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shelley</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>合计</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每月业绩</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2370,7 +2746,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -2473,6 +2849,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2480,7 +2893,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2678,6 +3091,84 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="57" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3046,13 +3537,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1028700</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3093,13 +3584,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>819150</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3140,13 +3631,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1009650</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>676275</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3187,13 +3678,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>771525</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3234,13 +3725,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1152525</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3345,6 +3836,53 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2162175" y="838200"/>
+          <a:ext cx="704850" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>781050</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="直接箭头连接符 14"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2162175" y="1781175"/>
           <a:ext cx="704850" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -3663,7 +4201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD317"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
@@ -10199,10 +10737,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H25"/>
+  <dimension ref="A3:H29"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -10258,38 +10796,59 @@
         <v>389</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
-      <c r="B16" s="49" t="s">
+    <row r="12" spans="1:8">
+      <c r="B12" s="101" t="s">
+        <v>522</v>
+      </c>
+      <c r="D12" s="49" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="B13" s="47" t="s">
+        <v>532</v>
+      </c>
+      <c r="D13" s="47" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="B14" s="47" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8">
+      <c r="B20" s="49" t="s">
         <v>273</v>
       </c>
-      <c r="D16" s="49" t="s">
+      <c r="D20" s="49" t="s">
         <v>274</v>
       </c>
-      <c r="F16" s="49" t="s">
+      <c r="F20" s="49" t="s">
         <v>280</v>
       </c>
-      <c r="H16" s="49" t="s">
+      <c r="H20" s="49" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="19" spans="2:6">
-      <c r="B19" s="49" t="s">
+    <row r="23" spans="2:8">
+      <c r="B23" s="49" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="22" spans="2:6">
-      <c r="B22" s="49" t="s">
+    <row r="26" spans="2:8">
+      <c r="B26" s="49" t="s">
         <v>276</v>
       </c>
-      <c r="D22" s="49" t="s">
+      <c r="D26" s="49" t="s">
         <v>277</v>
       </c>
-      <c r="F22" s="49" t="s">
+      <c r="F26" s="49" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="25" spans="2:6">
-      <c r="B25" s="47" t="s">
+    <row r="29" spans="2:8">
+      <c r="B29" s="47" t="s">
         <v>460</v>
       </c>
     </row>
@@ -10302,14 +10861,1027 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:Q70"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9" style="78"/>
+    <col min="2" max="2" width="10.25" style="78" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9" style="78"/>
+    <col min="5" max="5" width="12.5" style="78" customWidth="1"/>
+    <col min="6" max="6" width="15.5" style="78" customWidth="1"/>
+    <col min="7" max="7" width="16.5" style="78" customWidth="1"/>
+    <col min="8" max="8" width="11.625" style="78" customWidth="1"/>
+    <col min="9" max="9" width="14.25" style="78" customWidth="1"/>
+    <col min="10" max="10" width="10.625" style="78" customWidth="1"/>
+    <col min="11" max="11" width="16.875" style="78" customWidth="1"/>
+    <col min="12" max="12" width="14.375" style="78" customWidth="1"/>
+    <col min="13" max="13" width="10.125" style="78" customWidth="1"/>
+    <col min="14" max="14" width="12.75" style="78" customWidth="1"/>
+    <col min="15" max="16" width="9" style="78"/>
+    <col min="17" max="17" width="9.5" style="78" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9" style="78"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:17">
+      <c r="B4" s="78" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17">
+      <c r="B5" s="80" t="s">
+        <v>509</v>
+      </c>
+      <c r="C5" s="80" t="s">
+        <v>568</v>
+      </c>
+      <c r="D5" s="80" t="s">
+        <v>569</v>
+      </c>
+      <c r="E5" s="80" t="s">
+        <v>570</v>
+      </c>
+      <c r="F5" s="80" t="s">
+        <v>571</v>
+      </c>
+      <c r="G5" s="80" t="s">
+        <v>294</v>
+      </c>
+      <c r="H5" s="80" t="s">
+        <v>572</v>
+      </c>
+      <c r="I5" s="80" t="s">
+        <v>573</v>
+      </c>
+      <c r="J5" s="80" t="s">
+        <v>576</v>
+      </c>
+      <c r="K5" s="80" t="s">
+        <v>577</v>
+      </c>
+      <c r="L5" s="80" t="s">
+        <v>578</v>
+      </c>
+      <c r="M5" s="80" t="s">
+        <v>543</v>
+      </c>
+      <c r="N5" s="80" t="s">
+        <v>574</v>
+      </c>
+      <c r="O5" s="80" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17">
+      <c r="B6" s="78">
+        <v>1</v>
+      </c>
+      <c r="C6" s="78" t="s">
+        <v>513</v>
+      </c>
+      <c r="D6" s="78" t="s">
+        <v>515</v>
+      </c>
+      <c r="E6" s="78" t="s">
+        <v>517</v>
+      </c>
+      <c r="F6" s="78" t="s">
+        <v>536</v>
+      </c>
+      <c r="G6" s="78" t="s">
+        <v>510</v>
+      </c>
+      <c r="H6" s="78" t="s">
+        <v>552</v>
+      </c>
+      <c r="I6" s="78">
+        <v>65000</v>
+      </c>
+      <c r="J6" s="78">
+        <v>65000</v>
+      </c>
+      <c r="K6" s="79">
+        <v>44317</v>
+      </c>
+      <c r="L6" s="78" t="s">
+        <v>539</v>
+      </c>
+      <c r="M6" s="78" t="s">
+        <v>539</v>
+      </c>
+      <c r="N6" s="78" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17">
+      <c r="B7" s="78">
+        <v>2</v>
+      </c>
+      <c r="C7" s="78" t="s">
+        <v>516</v>
+      </c>
+      <c r="D7" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="E7" s="78" t="s">
+        <v>519</v>
+      </c>
+      <c r="F7" s="78" t="s">
+        <v>511</v>
+      </c>
+      <c r="G7" s="78" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="78" t="s">
+        <v>551</v>
+      </c>
+      <c r="I7" s="78">
+        <v>80000</v>
+      </c>
+      <c r="J7" s="78">
+        <v>80000</v>
+      </c>
+      <c r="K7" s="79">
+        <v>44317</v>
+      </c>
+      <c r="L7" s="78" t="s">
+        <v>539</v>
+      </c>
+      <c r="M7" s="78" t="s">
+        <v>539</v>
+      </c>
+      <c r="N7" s="78" t="s">
+        <v>580</v>
+      </c>
+      <c r="Q7" s="79"/>
+    </row>
+    <row r="8" spans="2:17">
+      <c r="B8" s="78">
+        <v>3</v>
+      </c>
+      <c r="C8" s="78" t="s">
+        <v>516</v>
+      </c>
+      <c r="D8" s="78" t="s">
+        <v>515</v>
+      </c>
+      <c r="E8" s="78" t="s">
+        <v>518</v>
+      </c>
+      <c r="F8" s="78" t="s">
+        <v>511</v>
+      </c>
+      <c r="G8" s="78" t="s">
+        <v>512</v>
+      </c>
+      <c r="H8" s="78" t="s">
+        <v>550</v>
+      </c>
+      <c r="I8" s="78">
+        <v>130000</v>
+      </c>
+      <c r="J8" s="78">
+        <v>130000</v>
+      </c>
+      <c r="K8" s="79">
+        <v>44348</v>
+      </c>
+      <c r="L8" s="78" t="s">
+        <v>539</v>
+      </c>
+      <c r="M8" s="78" t="s">
+        <v>539</v>
+      </c>
+      <c r="N8" s="78" t="s">
+        <v>564</v>
+      </c>
+      <c r="Q8" s="79"/>
+    </row>
+    <row r="9" spans="2:17">
+      <c r="B9" s="78">
+        <v>4</v>
+      </c>
+      <c r="C9" s="78" t="s">
+        <v>516</v>
+      </c>
+      <c r="D9" s="78" t="s">
+        <v>514</v>
+      </c>
+      <c r="E9" s="78" t="s">
+        <v>519</v>
+      </c>
+      <c r="F9" s="78" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="78" t="s">
+        <v>538</v>
+      </c>
+      <c r="H9" s="78" t="s">
+        <v>549</v>
+      </c>
+      <c r="I9" s="78">
+        <v>320000</v>
+      </c>
+      <c r="J9" s="78">
+        <v>250000</v>
+      </c>
+      <c r="K9" s="79">
+        <v>44348</v>
+      </c>
+      <c r="L9" s="78" t="s">
+        <v>540</v>
+      </c>
+      <c r="M9" s="78" t="s">
+        <v>544</v>
+      </c>
+      <c r="N9" s="78" t="s">
+        <v>564</v>
+      </c>
+      <c r="Q9" s="79"/>
+    </row>
+    <row r="10" spans="2:17">
+      <c r="B10" s="78">
+        <v>5</v>
+      </c>
+      <c r="C10" s="78" t="s">
+        <v>313</v>
+      </c>
+      <c r="D10" s="78" t="s">
+        <v>541</v>
+      </c>
+      <c r="E10" s="78" t="s">
+        <v>545</v>
+      </c>
+      <c r="F10" s="78" t="s">
+        <v>546</v>
+      </c>
+      <c r="G10" s="78" t="s">
+        <v>547</v>
+      </c>
+      <c r="H10" s="78" t="s">
+        <v>548</v>
+      </c>
+      <c r="I10" s="78">
+        <v>90000</v>
+      </c>
+      <c r="J10" s="78">
+        <v>18000</v>
+      </c>
+      <c r="K10" s="79">
+        <v>44348</v>
+      </c>
+      <c r="L10" s="78" t="s">
+        <v>542</v>
+      </c>
+      <c r="M10" s="78" t="s">
+        <v>553</v>
+      </c>
+      <c r="N10" s="78" t="s">
+        <v>581</v>
+      </c>
+      <c r="Q10" s="79"/>
+    </row>
+    <row r="11" spans="2:17">
+      <c r="B11" s="78">
+        <v>6</v>
+      </c>
+      <c r="C11" s="78" t="s">
+        <v>313</v>
+      </c>
+      <c r="D11" s="78" t="s">
+        <v>541</v>
+      </c>
+      <c r="E11" s="78" t="s">
+        <v>545</v>
+      </c>
+      <c r="F11" s="78" t="s">
+        <v>546</v>
+      </c>
+      <c r="G11" s="78" t="s">
+        <v>554</v>
+      </c>
+      <c r="H11" s="78" t="s">
+        <v>556</v>
+      </c>
+      <c r="I11" s="78">
+        <v>70000</v>
+      </c>
+      <c r="J11" s="78">
+        <v>14000</v>
+      </c>
+      <c r="K11" s="79">
+        <v>44348</v>
+      </c>
+      <c r="L11" s="78" t="s">
+        <v>542</v>
+      </c>
+      <c r="M11" s="78" t="s">
+        <v>553</v>
+      </c>
+      <c r="N11" s="78" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" ht="11.25" customHeight="1"/>
+    <row r="15" spans="2:17" ht="11.25" customHeight="1"/>
+    <row r="16" spans="2:17" ht="11.25" customHeight="1"/>
+    <row r="17" spans="2:12" ht="11.25" customHeight="1">
+      <c r="B17" s="78" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" ht="11.25" customHeight="1">
+      <c r="B18" s="96" t="s">
+        <v>537</v>
+      </c>
+      <c r="C18" s="96" t="s">
+        <v>567</v>
+      </c>
+      <c r="D18" s="96" t="s">
+        <v>579</v>
+      </c>
+      <c r="E18" s="96" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" ht="11.25" customHeight="1">
+      <c r="B19" s="95">
+        <v>1</v>
+      </c>
+      <c r="C19" s="95" t="s">
+        <v>520</v>
+      </c>
+      <c r="D19" s="95">
+        <v>35000</v>
+      </c>
+      <c r="E19" s="95">
+        <v>1</v>
+      </c>
+      <c r="I19" s="79"/>
+      <c r="J19" s="79"/>
+    </row>
+    <row r="20" spans="2:12" ht="11.25" customHeight="1">
+      <c r="B20" s="95">
+        <v>2</v>
+      </c>
+      <c r="C20" s="95" t="s">
+        <v>526</v>
+      </c>
+      <c r="D20" s="95">
+        <v>30000</v>
+      </c>
+      <c r="E20" s="95">
+        <v>1</v>
+      </c>
+      <c r="G20" s="81" t="s">
+        <v>584</v>
+      </c>
+      <c r="H20" s="82" t="s">
+        <v>588</v>
+      </c>
+      <c r="I20" s="103" t="s">
+        <v>589</v>
+      </c>
+      <c r="J20" s="103" t="s">
+        <v>590</v>
+      </c>
+      <c r="K20" s="82" t="s">
+        <v>591</v>
+      </c>
+      <c r="L20" s="83" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" ht="11.25" customHeight="1">
+      <c r="B21" s="95">
+        <v>3</v>
+      </c>
+      <c r="C21" s="95" t="s">
+        <v>521</v>
+      </c>
+      <c r="D21" s="95">
+        <v>80000</v>
+      </c>
+      <c r="E21" s="95">
+        <v>2</v>
+      </c>
+      <c r="G21" s="84" t="s">
+        <v>585</v>
+      </c>
+      <c r="H21" s="85">
+        <v>20</v>
+      </c>
+      <c r="I21" s="85">
+        <v>10</v>
+      </c>
+      <c r="J21" s="85">
+        <v>3</v>
+      </c>
+      <c r="K21" s="85">
+        <v>5</v>
+      </c>
+      <c r="L21" s="86"/>
+    </row>
+    <row r="22" spans="2:12" ht="11.25" customHeight="1">
+      <c r="B22" s="95">
+        <v>4</v>
+      </c>
+      <c r="C22" s="95" t="s">
+        <v>528</v>
+      </c>
+      <c r="D22" s="95">
+        <v>40000</v>
+      </c>
+      <c r="E22" s="95">
+        <v>3</v>
+      </c>
+      <c r="G22" s="84" t="s">
+        <v>586</v>
+      </c>
+      <c r="H22" s="85"/>
+      <c r="I22" s="85"/>
+      <c r="J22" s="85"/>
+      <c r="K22" s="85"/>
+      <c r="L22" s="86"/>
+    </row>
+    <row r="23" spans="2:12" ht="11.25" customHeight="1">
+      <c r="B23" s="95">
+        <v>5</v>
+      </c>
+      <c r="C23" s="95" t="s">
+        <v>529</v>
+      </c>
+      <c r="D23" s="95">
+        <v>40000</v>
+      </c>
+      <c r="E23" s="95">
+        <v>3</v>
+      </c>
+      <c r="G23" s="84" t="s">
+        <v>587</v>
+      </c>
+      <c r="H23" s="85"/>
+      <c r="I23" s="85"/>
+      <c r="J23" s="85"/>
+      <c r="K23" s="85"/>
+      <c r="L23" s="86"/>
+    </row>
+    <row r="24" spans="2:12" ht="11.25" customHeight="1">
+      <c r="B24" s="95">
+        <v>6</v>
+      </c>
+      <c r="C24" s="95" t="s">
+        <v>530</v>
+      </c>
+      <c r="D24" s="95">
+        <v>50000</v>
+      </c>
+      <c r="E24" s="95">
+        <v>3</v>
+      </c>
+      <c r="G24" s="84"/>
+      <c r="H24" s="85"/>
+      <c r="I24" s="85"/>
+      <c r="J24" s="85"/>
+      <c r="K24" s="85"/>
+      <c r="L24" s="86"/>
+    </row>
+    <row r="25" spans="2:12" ht="11.25" customHeight="1">
+      <c r="B25" s="95">
+        <v>7</v>
+      </c>
+      <c r="C25" s="95" t="s">
+        <v>539</v>
+      </c>
+      <c r="D25" s="95">
+        <v>250000</v>
+      </c>
+      <c r="E25" s="95">
+        <v>4</v>
+      </c>
+      <c r="G25" s="84"/>
+      <c r="H25" s="85"/>
+      <c r="I25" s="85"/>
+      <c r="J25" s="85"/>
+      <c r="K25" s="85"/>
+      <c r="L25" s="86"/>
+    </row>
+    <row r="26" spans="2:12" ht="11.25" customHeight="1">
+      <c r="B26" s="95">
+        <v>8</v>
+      </c>
+      <c r="C26" s="95" t="s">
+        <v>555</v>
+      </c>
+      <c r="D26" s="95">
+        <v>70000</v>
+      </c>
+      <c r="E26" s="95">
+        <v>4</v>
+      </c>
+      <c r="G26" s="84"/>
+      <c r="H26" s="85"/>
+      <c r="I26" s="85"/>
+      <c r="J26" s="85"/>
+      <c r="K26" s="85"/>
+      <c r="L26" s="86"/>
+    </row>
+    <row r="27" spans="2:12" ht="11.25" customHeight="1">
+      <c r="B27" s="95">
+        <v>9</v>
+      </c>
+      <c r="C27" s="95" t="s">
+        <v>521</v>
+      </c>
+      <c r="D27" s="95">
+        <v>18000</v>
+      </c>
+      <c r="E27" s="95">
+        <v>5</v>
+      </c>
+      <c r="G27" s="84"/>
+      <c r="H27" s="85"/>
+      <c r="I27" s="85"/>
+      <c r="J27" s="85"/>
+      <c r="K27" s="85"/>
+      <c r="L27" s="86"/>
+    </row>
+    <row r="28" spans="2:12" ht="11.25" customHeight="1">
+      <c r="B28" s="95">
+        <v>10</v>
+      </c>
+      <c r="C28" s="95" t="s">
+        <v>557</v>
+      </c>
+      <c r="D28" s="95">
+        <v>72000</v>
+      </c>
+      <c r="E28" s="95">
+        <v>5</v>
+      </c>
+      <c r="G28" s="84"/>
+      <c r="H28" s="85"/>
+      <c r="I28" s="85"/>
+      <c r="J28" s="85"/>
+      <c r="K28" s="85"/>
+      <c r="L28" s="86"/>
+    </row>
+    <row r="29" spans="2:12" ht="11.25" customHeight="1">
+      <c r="B29" s="95">
+        <v>11</v>
+      </c>
+      <c r="C29" s="95" t="s">
+        <v>558</v>
+      </c>
+      <c r="D29" s="95">
+        <v>14000</v>
+      </c>
+      <c r="E29" s="95">
+        <v>6</v>
+      </c>
+      <c r="G29" s="84"/>
+      <c r="H29" s="85"/>
+      <c r="I29" s="85"/>
+      <c r="J29" s="85"/>
+      <c r="K29" s="85"/>
+      <c r="L29" s="86"/>
+    </row>
+    <row r="30" spans="2:12" ht="11.25" customHeight="1">
+      <c r="B30" s="95">
+        <v>12</v>
+      </c>
+      <c r="C30" s="95" t="s">
+        <v>559</v>
+      </c>
+      <c r="D30" s="95">
+        <v>56000</v>
+      </c>
+      <c r="E30" s="95">
+        <v>6</v>
+      </c>
+      <c r="G30" s="84"/>
+      <c r="H30" s="85"/>
+      <c r="I30" s="85"/>
+      <c r="J30" s="85"/>
+      <c r="K30" s="85"/>
+      <c r="L30" s="86"/>
+    </row>
+    <row r="31" spans="2:12" ht="11.25" customHeight="1">
+      <c r="B31" s="85"/>
+      <c r="C31" s="85"/>
+      <c r="D31" s="85"/>
+      <c r="E31" s="85"/>
+      <c r="G31" s="87"/>
+      <c r="H31" s="88"/>
+      <c r="I31" s="88"/>
+      <c r="J31" s="88"/>
+      <c r="K31" s="88"/>
+      <c r="L31" s="89"/>
+    </row>
+    <row r="32" spans="2:12" ht="11.25" customHeight="1"/>
+    <row r="33" spans="2:14" ht="11.25" customHeight="1"/>
+    <row r="34" spans="2:14" ht="11.25" customHeight="1"/>
+    <row r="35" spans="2:14" ht="11.25" customHeight="1"/>
+    <row r="36" spans="2:14" ht="11.25" customHeight="1"/>
+    <row r="37" spans="2:14" ht="11.25" customHeight="1"/>
+    <row r="38" spans="2:14" ht="11.25" customHeight="1"/>
+    <row r="39" spans="2:14" ht="11.25" customHeight="1"/>
+    <row r="40" spans="2:14" ht="11.25" customHeight="1"/>
+    <row r="41" spans="2:14" ht="11.25" customHeight="1"/>
+    <row r="42" spans="2:14" ht="11.25" customHeight="1">
+      <c r="B42" s="100" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14" ht="11.25" customHeight="1"/>
+    <row r="44" spans="2:14" ht="11.25" customHeight="1"/>
+    <row r="45" spans="2:14" ht="11.25" customHeight="1"/>
+    <row r="46" spans="2:14" ht="11.25" customHeight="1"/>
+    <row r="47" spans="2:14">
+      <c r="B47" s="81"/>
+      <c r="C47" s="81"/>
+      <c r="D47" s="82"/>
+      <c r="E47" s="82"/>
+      <c r="F47" s="82"/>
+      <c r="G47" s="82"/>
+      <c r="H47" s="82"/>
+      <c r="I47" s="82"/>
+      <c r="J47" s="82"/>
+      <c r="K47" s="82"/>
+      <c r="L47" s="82"/>
+      <c r="M47" s="83"/>
+      <c r="N47" s="83"/>
+    </row>
+    <row r="48" spans="2:14">
+      <c r="B48" s="84"/>
+      <c r="C48" s="84"/>
+      <c r="D48" s="85"/>
+      <c r="E48" s="85"/>
+      <c r="F48" s="85"/>
+      <c r="G48" s="85"/>
+      <c r="H48" s="85"/>
+      <c r="I48" s="85"/>
+      <c r="J48" s="85"/>
+      <c r="K48" s="85"/>
+      <c r="L48" s="85"/>
+      <c r="M48" s="86"/>
+      <c r="N48" s="86"/>
+    </row>
+    <row r="49" spans="2:14">
+      <c r="B49" s="90"/>
+      <c r="C49" s="88"/>
+      <c r="D49" s="88"/>
+      <c r="E49" s="88"/>
+      <c r="F49" s="88"/>
+      <c r="G49" s="88"/>
+      <c r="H49" s="88"/>
+      <c r="I49" s="88"/>
+      <c r="J49" s="88"/>
+      <c r="K49" s="88"/>
+      <c r="L49" s="88"/>
+      <c r="M49" s="89"/>
+      <c r="N49" s="86"/>
+    </row>
+    <row r="50" spans="2:14">
+      <c r="B50" s="91"/>
+      <c r="C50" s="85"/>
+      <c r="D50" s="85"/>
+      <c r="E50" s="85"/>
+      <c r="F50" s="85"/>
+      <c r="G50" s="85"/>
+      <c r="H50" s="85"/>
+      <c r="I50" s="85"/>
+      <c r="J50" s="85"/>
+      <c r="K50" s="85"/>
+      <c r="L50" s="85"/>
+      <c r="M50" s="85"/>
+      <c r="N50" s="86"/>
+    </row>
+    <row r="51" spans="2:14">
+      <c r="B51" s="91"/>
+      <c r="C51" s="102" t="s">
+        <v>583</v>
+      </c>
+      <c r="D51" s="96" t="s">
+        <v>593</v>
+      </c>
+      <c r="E51" s="99" t="s">
+        <v>523</v>
+      </c>
+      <c r="F51" s="98" t="s">
+        <v>560</v>
+      </c>
+      <c r="G51" s="97" t="s">
+        <v>524</v>
+      </c>
+      <c r="H51" s="99" t="s">
+        <v>561</v>
+      </c>
+      <c r="I51" s="96" t="s">
+        <v>562</v>
+      </c>
+      <c r="J51" s="95"/>
+      <c r="K51" s="95"/>
+      <c r="L51" s="95"/>
+      <c r="M51" s="85"/>
+      <c r="N51" s="86"/>
+    </row>
+    <row r="52" spans="2:14">
+      <c r="B52" s="91"/>
+      <c r="C52" s="94" t="s">
+        <v>525</v>
+      </c>
+      <c r="D52" s="82"/>
+      <c r="E52" s="82"/>
+      <c r="F52" s="82"/>
+      <c r="G52" s="82"/>
+      <c r="H52" s="82"/>
+      <c r="I52" s="82"/>
+      <c r="J52" s="82"/>
+      <c r="K52" s="82"/>
+      <c r="L52" s="82"/>
+      <c r="M52" s="82"/>
+      <c r="N52" s="83"/>
+    </row>
+    <row r="53" spans="2:14">
+      <c r="B53" s="91"/>
+      <c r="C53" s="84"/>
+      <c r="D53" s="85"/>
+      <c r="E53" s="85"/>
+      <c r="F53" s="85"/>
+      <c r="G53" s="85"/>
+      <c r="H53" s="85"/>
+      <c r="I53" s="85"/>
+      <c r="J53" s="85"/>
+      <c r="K53" s="85"/>
+      <c r="L53" s="85"/>
+      <c r="M53" s="85"/>
+      <c r="N53" s="86"/>
+    </row>
+    <row r="54" spans="2:14">
+      <c r="B54" s="91"/>
+      <c r="C54" s="84"/>
+      <c r="D54" s="85"/>
+      <c r="E54" s="85"/>
+      <c r="F54" s="85"/>
+      <c r="G54" s="85"/>
+      <c r="H54" s="85"/>
+      <c r="I54" s="85"/>
+      <c r="J54" s="85"/>
+      <c r="K54" s="85"/>
+      <c r="L54" s="85"/>
+      <c r="M54" s="85"/>
+      <c r="N54" s="86"/>
+    </row>
+    <row r="55" spans="2:14">
+      <c r="B55" s="92"/>
+      <c r="C55" s="84"/>
+      <c r="D55" s="85"/>
+      <c r="E55" s="85"/>
+      <c r="F55" s="85"/>
+      <c r="G55" s="85"/>
+      <c r="H55" s="85"/>
+      <c r="I55" s="85"/>
+      <c r="J55" s="85"/>
+      <c r="K55" s="85"/>
+      <c r="L55" s="85"/>
+      <c r="M55" s="85"/>
+      <c r="N55" s="86"/>
+    </row>
+    <row r="56" spans="2:14">
+      <c r="B56" s="91"/>
+      <c r="C56" s="84"/>
+      <c r="D56" s="85"/>
+      <c r="E56" s="85"/>
+      <c r="F56" s="85"/>
+      <c r="G56" s="85"/>
+      <c r="H56" s="85"/>
+      <c r="I56" s="85"/>
+      <c r="J56" s="85"/>
+      <c r="K56" s="85"/>
+      <c r="L56" s="85"/>
+      <c r="M56" s="85"/>
+      <c r="N56" s="86"/>
+    </row>
+    <row r="57" spans="2:14">
+      <c r="B57" s="91"/>
+      <c r="C57" s="84"/>
+      <c r="D57" s="85"/>
+      <c r="E57" s="85"/>
+      <c r="F57" s="85"/>
+      <c r="G57" s="85"/>
+      <c r="H57" s="85"/>
+      <c r="I57" s="85"/>
+      <c r="J57" s="85"/>
+      <c r="K57" s="85"/>
+      <c r="L57" s="85"/>
+      <c r="M57" s="85"/>
+      <c r="N57" s="86"/>
+    </row>
+    <row r="58" spans="2:14">
+      <c r="B58" s="91"/>
+      <c r="C58" s="84"/>
+      <c r="D58" s="85"/>
+      <c r="E58" s="85"/>
+      <c r="F58" s="85"/>
+      <c r="G58" s="85"/>
+      <c r="H58" s="85"/>
+      <c r="I58" s="85"/>
+      <c r="J58" s="85"/>
+      <c r="K58" s="85"/>
+      <c r="L58" s="85"/>
+      <c r="M58" s="85"/>
+      <c r="N58" s="86"/>
+    </row>
+    <row r="59" spans="2:14">
+      <c r="B59" s="91"/>
+      <c r="C59" s="84"/>
+      <c r="D59" s="85"/>
+      <c r="E59" s="85"/>
+      <c r="F59" s="85"/>
+      <c r="G59" s="85"/>
+      <c r="H59" s="85"/>
+      <c r="I59" s="85"/>
+      <c r="J59" s="85"/>
+      <c r="K59" s="85"/>
+      <c r="L59" s="85"/>
+      <c r="M59" s="85"/>
+      <c r="N59" s="86"/>
+    </row>
+    <row r="60" spans="2:14">
+      <c r="B60" s="91"/>
+      <c r="C60" s="84"/>
+      <c r="D60" s="85"/>
+      <c r="E60" s="85"/>
+      <c r="F60" s="85"/>
+      <c r="G60" s="85"/>
+      <c r="H60" s="85"/>
+      <c r="I60" s="85"/>
+      <c r="J60" s="85"/>
+      <c r="K60" s="85"/>
+      <c r="L60" s="85"/>
+      <c r="M60" s="85"/>
+      <c r="N60" s="86"/>
+    </row>
+    <row r="61" spans="2:14">
+      <c r="B61" s="91"/>
+      <c r="C61" s="84"/>
+      <c r="D61" s="85"/>
+      <c r="E61" s="85"/>
+      <c r="F61" s="85"/>
+      <c r="G61" s="85"/>
+      <c r="H61" s="85"/>
+      <c r="I61" s="85"/>
+      <c r="J61" s="85"/>
+      <c r="K61" s="85"/>
+      <c r="L61" s="85"/>
+      <c r="M61" s="85"/>
+      <c r="N61" s="86"/>
+    </row>
+    <row r="62" spans="2:14">
+      <c r="B62" s="91"/>
+      <c r="C62" s="84"/>
+      <c r="D62" s="85"/>
+      <c r="E62" s="85"/>
+      <c r="F62" s="85"/>
+      <c r="G62" s="85"/>
+      <c r="H62" s="85"/>
+      <c r="I62" s="85"/>
+      <c r="J62" s="85"/>
+      <c r="K62" s="85"/>
+      <c r="L62" s="85"/>
+      <c r="M62" s="85"/>
+      <c r="N62" s="86"/>
+    </row>
+    <row r="63" spans="2:14">
+      <c r="B63" s="91"/>
+      <c r="C63" s="84"/>
+      <c r="D63" s="85"/>
+      <c r="E63" s="85"/>
+      <c r="F63" s="85"/>
+      <c r="G63" s="85"/>
+      <c r="H63" s="85"/>
+      <c r="I63" s="85"/>
+      <c r="J63" s="85"/>
+      <c r="K63" s="85"/>
+      <c r="L63" s="85"/>
+      <c r="M63" s="85"/>
+      <c r="N63" s="86"/>
+    </row>
+    <row r="64" spans="2:14">
+      <c r="B64" s="91"/>
+      <c r="C64" s="84"/>
+      <c r="D64" s="85"/>
+      <c r="E64" s="85"/>
+      <c r="F64" s="85"/>
+      <c r="G64" s="85"/>
+      <c r="H64" s="85"/>
+      <c r="I64" s="85"/>
+      <c r="J64" s="85"/>
+      <c r="K64" s="85"/>
+      <c r="L64" s="85"/>
+      <c r="M64" s="85"/>
+      <c r="N64" s="86"/>
+    </row>
+    <row r="65" spans="2:14">
+      <c r="B65" s="91"/>
+      <c r="C65" s="84"/>
+      <c r="D65" s="85"/>
+      <c r="E65" s="85"/>
+      <c r="F65" s="85"/>
+      <c r="G65" s="85"/>
+      <c r="H65" s="85"/>
+      <c r="I65" s="85"/>
+      <c r="J65" s="85"/>
+      <c r="K65" s="85"/>
+      <c r="L65" s="85"/>
+      <c r="M65" s="85"/>
+      <c r="N65" s="86"/>
+    </row>
+    <row r="66" spans="2:14">
+      <c r="B66" s="91"/>
+      <c r="C66" s="84"/>
+      <c r="D66" s="85"/>
+      <c r="E66" s="85"/>
+      <c r="F66" s="85"/>
+      <c r="G66" s="85"/>
+      <c r="H66" s="85"/>
+      <c r="I66" s="85"/>
+      <c r="J66" s="85"/>
+      <c r="K66" s="85"/>
+      <c r="L66" s="85"/>
+      <c r="M66" s="85"/>
+      <c r="N66" s="86"/>
+    </row>
+    <row r="67" spans="2:14">
+      <c r="B67" s="91"/>
+      <c r="C67" s="84"/>
+      <c r="D67" s="85"/>
+      <c r="E67" s="85"/>
+      <c r="F67" s="85"/>
+      <c r="G67" s="85"/>
+      <c r="H67" s="85"/>
+      <c r="I67" s="85"/>
+      <c r="J67" s="85"/>
+      <c r="K67" s="85"/>
+      <c r="L67" s="85"/>
+      <c r="M67" s="85"/>
+      <c r="N67" s="86"/>
+    </row>
+    <row r="68" spans="2:14">
+      <c r="B68" s="91"/>
+      <c r="C68" s="84"/>
+      <c r="D68" s="85"/>
+      <c r="E68" s="85"/>
+      <c r="F68" s="85"/>
+      <c r="G68" s="85"/>
+      <c r="H68" s="85"/>
+      <c r="I68" s="85"/>
+      <c r="J68" s="85"/>
+      <c r="K68" s="85"/>
+      <c r="L68" s="85"/>
+      <c r="M68" s="85"/>
+      <c r="N68" s="86"/>
+    </row>
+    <row r="69" spans="2:14">
+      <c r="B69" s="91"/>
+      <c r="C69" s="84"/>
+      <c r="D69" s="85"/>
+      <c r="E69" s="85"/>
+      <c r="F69" s="85"/>
+      <c r="G69" s="85"/>
+      <c r="H69" s="85"/>
+      <c r="I69" s="85"/>
+      <c r="J69" s="85"/>
+      <c r="K69" s="85"/>
+      <c r="L69" s="85"/>
+      <c r="M69" s="85"/>
+      <c r="N69" s="86"/>
+    </row>
+    <row r="70" spans="2:14">
+      <c r="B70" s="93"/>
+      <c r="C70" s="87"/>
+      <c r="D70" s="88"/>
+      <c r="E70" s="88"/>
+      <c r="F70" s="88"/>
+      <c r="G70" s="88"/>
+      <c r="H70" s="88"/>
+      <c r="I70" s="88"/>
+      <c r="J70" s="88"/>
+      <c r="K70" s="88"/>
+      <c r="L70" s="88"/>
+      <c r="M70" s="88"/>
+      <c r="N70" s="89"/>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>